<commit_message>
MILESTONE: distritos split by concept
</commit_message>
<xml_diff>
--- a/static/menciones_por_lista.xlsx
+++ b/static/menciones_por_lista.xlsx
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>largo</t>
+          <t>lista</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -461,8 +461,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>119575</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A PULSO, POR EL BUEN VIVIR </t>
+        </is>
       </c>
       <c r="B2" t="n">
         <v>55</v>
@@ -478,8 +480,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>5031646</v>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>APRUEBO DIGNIDAD</t>
+        </is>
       </c>
       <c r="B3" t="n">
         <v>677</v>
@@ -495,8 +499,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>44944</v>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ARICA SIEMPRE ARICA </t>
+        </is>
       </c>
       <c r="B4" t="n">
         <v>4</v>
@@ -512,8 +518,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>147605</v>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>ASAMBLEA CONSTITUYENTE ATACAMA</t>
+        </is>
       </c>
       <c r="B5" t="n">
         <v>65</v>
@@ -529,8 +537,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>583864</v>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ASAMBLEA POPULAR CONSTITUYENTE </t>
+        </is>
       </c>
       <c r="B6" t="n">
         <v>104</v>
@@ -546,8 +556,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>59103</v>
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ASAMBLEA POPULAR POR LA DIGNIDAD </t>
+        </is>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -563,8 +575,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>124556</v>
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AUTONOMIA SOCIAL Y SINDICAL TARAPACA </t>
+        </is>
       </c>
       <c r="B8" t="n">
         <v>16</v>
@@ -580,8 +594,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>33504</v>
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BIOBIO SIN PARTIDOS </t>
+        </is>
       </c>
       <c r="B9" t="n">
         <v>9</v>
@@ -597,8 +613,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>13599</v>
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CABILDO AUTOCONVOCADO </t>
+        </is>
       </c>
       <c r="B10" t="n">
         <v>0</v>
@@ -614,8 +632,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>364210</v>
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>CANDIDATURA INDEPENDIENTE</t>
+        </is>
       </c>
       <c r="B11" t="n">
         <v>69</v>
@@ -631,8 +651,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>44210</v>
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CHILE INDEPENDIENTE </t>
+        </is>
       </c>
       <c r="B12" t="n">
         <v>5</v>
@@ -648,8 +670,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>194836</v>
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>CIUDADANOS CRISTIANOS</t>
+        </is>
       </c>
       <c r="B13" t="n">
         <v>29</v>
@@ -665,8 +689,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>50758</v>
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">COMUNIDAD INDEPENDIENTE DE MAULE </t>
+        </is>
       </c>
       <c r="B14" t="n">
         <v>7</v>
@@ -682,8 +708,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>48042</v>
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">COMUNIDAD INDEPENDIENTE VENSEREMOS </t>
+        </is>
       </c>
       <c r="B15" t="n">
         <v>5</v>
@@ -699,8 +727,10 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>113741</v>
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">COORDINADORA SOCIAL DE MAGALLANES </t>
+        </is>
       </c>
       <c r="B16" t="n">
         <v>22</v>
@@ -716,8 +746,10 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>174021</v>
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CORRIENTES INDEPENDIENTES </t>
+        </is>
       </c>
       <c r="B17" t="n">
         <v>67</v>
@@ -733,8 +765,10 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>39800</v>
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DECISION CIUDADANA </t>
+        </is>
       </c>
       <c r="B18" t="n">
         <v>32</v>
@@ -750,8 +784,10 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>100216</v>
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ELIGE LA LISTA DEL PUEBLO </t>
+        </is>
       </c>
       <c r="B19" t="n">
         <v>11</v>
@@ -767,8 +803,10 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>61732</v>
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ENERGIA INDEPENDIENTE </t>
+        </is>
       </c>
       <c r="B20" t="n">
         <v>12</v>
@@ -784,8 +822,10 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>85236</v>
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FUERZA SOCIAL DE ÑUBLE, LA LISTA DEL PUEBLO </t>
+        </is>
       </c>
       <c r="B21" t="n">
         <v>13</v>
@@ -801,8 +841,10 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
-        <v>38419</v>
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">INDEPENDIENTES COMO TU </t>
+        </is>
       </c>
       <c r="B22" t="n">
         <v>14</v>
@@ -818,8 +860,10 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
-        <v>42339</v>
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">INDEPENDIENTES CON CHILE </t>
+        </is>
       </c>
       <c r="B23" t="n">
         <v>1</v>
@@ -835,8 +879,10 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>51125</v>
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">INDEPENDIENTES DE TARAPACA </t>
+        </is>
       </c>
       <c r="B24" t="n">
         <v>28</v>
@@ -852,8 +898,10 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
-        <v>145557</v>
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">INDEPENDIENTES DE ÑUBLE POR LA NUEVA CONSTITUCION </t>
+        </is>
       </c>
       <c r="B25" t="n">
         <v>18</v>
@@ -869,8 +917,10 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
-        <v>115424</v>
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>INDEPENDIENTES DEL APRUEBO REGION COQUIMBO</t>
+        </is>
       </c>
       <c r="B26" t="n">
         <v>18</v>
@@ -886,8 +936,10 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
-        <v>98094</v>
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">INDEPENDIENTES DEL BIOBIO POR UNA NUEVA CONSTITUCION </t>
+        </is>
       </c>
       <c r="B27" t="n">
         <v>30</v>
@@ -903,8 +955,10 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
-        <v>72071</v>
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">INDEPENDIENTES DEL NORTE GRANDE POR UNA NUEVA CONSTITUCION </t>
+        </is>
       </c>
       <c r="B28" t="n">
         <v>8</v>
@@ -920,8 +974,10 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
-        <v>86334</v>
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">INDEPENDIENTES DISTRITO 6 + LISTA DEL PUEBLO </t>
+        </is>
       </c>
       <c r="B29" t="n">
         <v>8</v>
@@ -937,8 +993,10 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
-        <v>317765</v>
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">INDEPENDIENTES NUEVA CONSTITUCION </t>
+        </is>
       </c>
       <c r="B30" t="n">
         <v>25</v>
@@ -954,8 +1012,10 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
-        <v>2826125</v>
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">INDEPENDIENTES POR LA NUEVA CONSTITUCION </t>
+        </is>
       </c>
       <c r="B31" t="n">
         <v>240</v>
@@ -971,8 +1031,10 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n">
-        <v>20592</v>
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">INDEPENDIENTES POR LA REGION DE COQUIMBO </t>
+        </is>
       </c>
       <c r="B32" t="n">
         <v>9</v>
@@ -988,8 +1050,10 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n">
-        <v>1688089</v>
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">INDEPENDIENTES POR UNA NUEVA CONSTITUCION </t>
+        </is>
       </c>
       <c r="B33" t="n">
         <v>144</v>
@@ -1005,8 +1069,10 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n">
-        <v>70979</v>
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">INDEPENDIENTES SIN PADRINOS </t>
+        </is>
       </c>
       <c r="B34" t="n">
         <v>4</v>
@@ -1022,8 +1088,10 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n">
-        <v>191694</v>
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">INDEPENDIENTES Y MOVIMIENTOS SOCIALES DEL APRUEBO </t>
+        </is>
       </c>
       <c r="B35" t="n">
         <v>30</v>
@@ -1039,8 +1107,10 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="n">
-        <v>173389</v>
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">INSULARES E INDEPENDIENTES </t>
+        </is>
       </c>
       <c r="B36" t="n">
         <v>36</v>
@@ -1056,8 +1126,10 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="n">
-        <v>118075</v>
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>LA LISTA DEL PUEBLO</t>
+        </is>
       </c>
       <c r="B37" t="n">
         <v>10</v>
@@ -1073,8 +1145,10 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
-        <v>716990</v>
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LA LISTA DEL PUEBLO </t>
+        </is>
       </c>
       <c r="B38" t="n">
         <v>80</v>
@@ -1090,8 +1164,10 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="n">
-        <v>75815</v>
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LA LISTA DEL PUEBLO 100% INDEPENDIENTES </t>
+        </is>
       </c>
       <c r="B39" t="n">
         <v>4</v>
@@ -1107,8 +1183,10 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="n">
-        <v>111886</v>
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LA LISTA DEL PUEBLO DISTRITO 12 </t>
+        </is>
       </c>
       <c r="B40" t="n">
         <v>7</v>
@@ -1124,8 +1202,10 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="n">
-        <v>107130</v>
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LA LISTA DEL PUEBLO DISTRITO 14 </t>
+        </is>
       </c>
       <c r="B41" t="n">
         <v>10</v>
@@ -1141,8 +1221,10 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="n">
-        <v>123228</v>
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LA LISTA DEL PUEBLO DISTRITO 9 </t>
+        </is>
       </c>
       <c r="B42" t="n">
         <v>7</v>
@@ -1158,8 +1240,10 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="n">
-        <v>87525</v>
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LA LISTA DEL PUEBLO MAULE SUR </t>
+        </is>
       </c>
       <c r="B43" t="n">
         <v>5</v>
@@ -1175,8 +1259,10 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="n">
-        <v>5567466</v>
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>LISTA DEL APRUEBO</t>
+        </is>
       </c>
       <c r="B44" t="n">
         <v>948</v>
@@ -1192,8 +1278,10 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="n">
-        <v>45380</v>
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LISTA DEL PUEBLO TRANSFORMANDO DESDE EL WILLI </t>
+        </is>
       </c>
       <c r="B45" t="n">
         <v>4</v>
@@ -1209,8 +1297,10 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="n">
-        <v>162404</v>
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LISTA DEL PUEBLO – MOVIMIENTO TERRITORIAL CONSTITUYENTE </t>
+        </is>
       </c>
       <c r="B46" t="n">
         <v>58</v>
@@ -1226,8 +1316,10 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="n">
-        <v>37463</v>
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LISTA DEL PUEBLO-RIOS INDEPENDIENTES </t>
+        </is>
       </c>
       <c r="B47" t="n">
         <v>15</v>
@@ -1243,8 +1335,10 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="n">
-        <v>11733</v>
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LISTA INDEPENDIENTE PARTO SOCIAL </t>
+        </is>
       </c>
       <c r="B48" t="n">
         <v>6</v>
@@ -1260,8 +1354,10 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="n">
-        <v>71659</v>
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LISTA POR LA JUSTICIA SOCIAL </t>
+        </is>
       </c>
       <c r="B49" t="n">
         <v>7</v>
@@ -1277,8 +1373,10 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="n">
-        <v>269208</v>
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LISTA SOCIAL PODER CONSTITUYENTE A TODA COSTA </t>
+        </is>
       </c>
       <c r="B50" t="n">
         <v>54</v>
@@ -1294,8 +1392,10 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="n">
-        <v>76419</v>
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MAGALLANICOS NO NEUTRALES </t>
+        </is>
       </c>
       <c r="B51" t="n">
         <v>6</v>
@@ -1311,8 +1411,10 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="n">
-        <v>87592</v>
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MOVIMIENTO INDEPENDIENTES DEL NORTE </t>
+        </is>
       </c>
       <c r="B52" t="n">
         <v>30</v>
@@ -1328,8 +1430,10 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="n">
-        <v>48633</v>
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MOVIMIENTO SOCIAL CONSTITUYENTE / LA LISTA DEL PUEBLO </t>
+        </is>
       </c>
       <c r="B53" t="n">
         <v>42</v>
@@ -1345,8 +1449,10 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="n">
-        <v>88020</v>
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MOVIMIENTO SOCIAL LA LISTA DEL PUEBLO </t>
+        </is>
       </c>
       <c r="B54" t="n">
         <v>5</v>
@@ -1362,8 +1468,10 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="n">
-        <v>254614</v>
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MOVIMIENTOS SOCIALES : UNIDAD DE INDEPENDIENTES </t>
+        </is>
       </c>
       <c r="B55" t="n">
         <v>65</v>
@@ -1379,8 +1487,10 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="n">
-        <v>35566</v>
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MOVIMIENTOS SOCIALES AUTONOMOS </t>
+        </is>
       </c>
       <c r="B56" t="n">
         <v>6</v>
@@ -1396,8 +1506,10 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="n">
-        <v>32176</v>
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MOVIMIENTOS SOCIALES INDEPENDIENTES </t>
+        </is>
       </c>
       <c r="B57" t="n">
         <v>8</v>
@@ -1413,8 +1525,10 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="n">
-        <v>138510</v>
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MOVIMIENTOS SOCIALES PLURINACIONALES E INDEPENDIENTES </t>
+        </is>
       </c>
       <c r="B58" t="n">
         <v>12</v>
@@ -1430,8 +1544,10 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="n">
-        <v>333455</v>
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NOBLES HIJXOS DE TARAPACA </t>
+        </is>
       </c>
       <c r="B59" t="n">
         <v>50</v>
@@ -1447,8 +1563,10 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="n">
-        <v>80628</v>
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NUESTRAS VOCES </t>
+        </is>
       </c>
       <c r="B60" t="n">
         <v>16</v>
@@ -1464,8 +1582,10 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="n">
-        <v>427808</v>
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ORGANIZACIONES SOCIALES Y TERRITORIALES DEL WALLMAPU </t>
+        </is>
       </c>
       <c r="B61" t="n">
         <v>121</v>
@@ -1481,8 +1601,10 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="n">
-        <v>480363</v>
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>PARTIDO DE TRABAJADORES REVOLUCIONARIOS</t>
+        </is>
       </c>
       <c r="B62" t="n">
         <v>53</v>
@@ -1498,8 +1620,10 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="n">
-        <v>815085</v>
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>PARTIDO ECOLOGISTA VERDE</t>
+        </is>
       </c>
       <c r="B63" t="n">
         <v>390</v>
@@ -1515,8 +1639,10 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="n">
-        <v>44964</v>
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>PARTIDO HUMANISTA</t>
+        </is>
       </c>
       <c r="B64" t="n">
         <v>5</v>
@@ -1532,8 +1658,10 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="n">
-        <v>394615</v>
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>PARTIDO UNION PATRIOTICA</t>
+        </is>
       </c>
       <c r="B65" t="n">
         <v>81</v>
@@ -1549,8 +1677,10 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="n">
-        <v>2787</v>
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PATAGONIA SOMOS TODOS </t>
+        </is>
       </c>
       <c r="B66" t="n">
         <v>0</v>
@@ -1566,8 +1696,10 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="n">
-        <v>21800</v>
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PUEBLO UNIDO TARAPACA </t>
+        </is>
       </c>
       <c r="B67" t="n">
         <v>4</v>
@@ -1583,8 +1715,10 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="n">
-        <v>169470</v>
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">REGIONALISMO CIUDADANO INDEPENDIENTE </t>
+        </is>
       </c>
       <c r="B68" t="n">
         <v>24</v>
@@ -1600,8 +1734,10 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="n">
-        <v>21345</v>
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">REPUBLICA DE LOS INDEPENDIENTES DE MAGALLANES </t>
+        </is>
       </c>
       <c r="B69" t="n">
         <v>3</v>
@@ -1617,8 +1753,10 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="n">
-        <v>44435</v>
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SEXTA UNIDA </t>
+        </is>
       </c>
       <c r="B70" t="n">
         <v>14</v>
@@ -1634,8 +1772,10 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="n">
-        <v>31710</v>
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SOBERANIA CIUDADANA </t>
+        </is>
       </c>
       <c r="B71" t="n">
         <v>3</v>
@@ -1651,8 +1791,10 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="n">
-        <v>16103</v>
+      <c r="A72" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMATE AHORA </t>
+        </is>
       </c>
       <c r="B72" t="n">
         <v>0</v>
@@ -1668,8 +1810,10 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="n">
-        <v>3580523</v>
+      <c r="A73" s="1" t="inlineStr">
+        <is>
+          <t>VAMOS POR CHILE</t>
+        </is>
       </c>
       <c r="B73" t="n">
         <v>423</v>
@@ -1685,8 +1829,10 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="n">
-        <v>41589</v>
+      <c r="A74" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">VOCES CONSTITUYENTES </t>
+        </is>
       </c>
       <c r="B74" t="n">
         <v>15</v>

</xml_diff>